<commit_message>
Resolved merge conflict by keeping local changes
</commit_message>
<xml_diff>
--- a/results/baseline_CNN_results.xlsx
+++ b/results/baseline_CNN_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,45 +444,40 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Output</t>
+          <t>Split</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Resolution</t>
+          <t>nº samples</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>nº samples</t>
+          <t>Batch size</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Batch size</t>
+          <t>Epochs</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Epochs</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Date</t>
+          <t>Time</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Duration</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
-        <is>
-          <t>Duration</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
         <is>
           <t>Loss</t>
         </is>
@@ -490,14 +485,14 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>10.37964995798412</v>
+        <v>5.795400282503119</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>lst, ndvi, label, month</t>
+          <t>lst, no label</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -507,35 +502,32 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>wt</t>
+          <t>random</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>256</v>
+        <v>955</v>
       </c>
       <c r="G2" t="n">
-        <v>955</v>
+        <v>32</v>
       </c>
       <c r="H2" t="n">
-        <v>128</v>
-      </c>
-      <c r="I2" t="n">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2024-11-12</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>16:18:58</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>43.54</v>
-      </c>
-      <c r="M2" t="inlineStr">
+          <t>11:32:36</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>466.92</v>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>RMSE</t>
         </is>

</xml_diff>